<commit_message>
Tercera version de exportar a PDF
</commit_message>
<xml_diff>
--- a/datosMantenimiento1.xlsx
+++ b/datosMantenimiento1.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
@@ -450,27 +450,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col width="23" customWidth="1" min="1" max="17"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
-    <col width="23" customWidth="1" min="3" max="3"/>
-    <col width="23" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
-    <col width="23" customWidth="1" min="7" max="7"/>
-    <col width="23" customWidth="1" min="8" max="8"/>
-    <col width="23" customWidth="1" min="9" max="9"/>
-    <col width="23" customWidth="1" min="10" max="10"/>
-    <col width="23" customWidth="1" min="11" max="11"/>
-    <col width="23" customWidth="1" min="12" max="12"/>
-    <col width="23" customWidth="1" min="13" max="13"/>
-    <col width="23" customWidth="1" min="14" max="14"/>
-    <col width="23" customWidth="1" min="15" max="15"/>
-    <col width="23" customWidth="1" min="16" max="16"/>
-    <col width="23" customWidth="1" min="17" max="17"/>
-    <col width="23" customWidth="1" min="18" max="18"/>
-    <col width="23" customWidth="1" min="19" max="19"/>
-    <col width="23" customWidth="1" min="20" max="20"/>
-    <col width="23" customWidth="1" min="21" max="21"/>
+    <col width="24" customWidth="1" min="1" max="17"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="7" max="7"/>
+    <col width="24" customWidth="1" min="8" max="8"/>
+    <col width="24" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="10" max="10"/>
+    <col width="24" customWidth="1" min="11" max="11"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
+    <col width="24" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="14" max="14"/>
+    <col width="24" customWidth="1" min="15" max="15"/>
+    <col width="24" customWidth="1" min="16" max="16"/>
+    <col width="24" customWidth="1" min="17" max="17"/>
+    <col width="24" customWidth="1" min="18" max="18"/>
+    <col width="24" customWidth="1" min="19" max="19"/>
+    <col width="24" customWidth="1" min="20" max="20"/>
+    <col width="24" customWidth="1" min="21" max="21"/>
+    <col width="24" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -553,62 +554,62 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>1 DE ENERO DE 2000</t>
+          <t>tyrtuy</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CALI</t>
+          <t>tyrty</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>CHIPICHAPE</t>
+          <t>tytry</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>7777</t>
+          <t>efdghdfgdg</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>SALA DE VENTAS</t>
+          <t>dghdfh</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>JUAN PEREZ</t>
+          <t>dghdfh</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>98888888</t>
+          <t>567</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>LAPTOP</t>
+          <t>dgh</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>dhdf</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>440 G0</t>
+          <t>dfhdfh</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>5CG343435</t>
+          <t>dhdfh</t>
         </is>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>ML0001</t>
+          <t>dfgh</t>
         </is>
       </c>
       <c r="M2" s="2" t="inlineStr">
@@ -633,757 +634,880 @@
       </c>
       <c r="Q2" s="2" t="inlineStr">
         <is>
-          <t>LG</t>
+          <t>dghdfh</t>
         </is>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>II5I5I56</t>
+          <t>dfhdfhdf</t>
         </is>
       </c>
       <c r="S2" s="2" t="inlineStr">
         <is>
-          <t>ML2323</t>
+          <t>dhdfh</t>
         </is>
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>NINGUN ACCESOSORIO</t>
+          <t>Guaya, Maleta, Teclado</t>
         </is>
       </c>
       <c r="U2" s="2" t="inlineStr">
         <is>
-          <t>El usuario no se encuentra presente al momento de la toma de inventario.</t>
+          <t>Hub USB</t>
+        </is>
+      </c>
+      <c r="V2" s="2" t="inlineStr">
+        <is>
+          <t>sin mas accesorios</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>EFSFEF</t>
+          <t>fgmnvc</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>ASDFADF</t>
+          <t>mguiouioyuio</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>ASDAG</t>
+          <t>yioyuio</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>4435</t>
+          <t>yioyui</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>DSFDSF</t>
+          <t>oyioyuio</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>EREWYTEYUTURTYU</t>
+          <t>yuioyuio</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>34545664</t>
+          <t>yioyio</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>WEREWR</t>
+          <t>yioyi</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>WER</t>
+          <t>yioyui</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>EWR345</t>
+          <t>yioyi</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>DR435</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>TERTT</t>
+          <t>yioyi</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>yioyio</t>
         </is>
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>WEER</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
-          <t>34EREW</t>
+          <t>512 GB</t>
         </is>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>SDFE45</t>
+          <t>16 GB</t>
         </is>
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>WERRWRE</t>
+          <t>Intel Core i5 12th</t>
         </is>
       </c>
       <c r="Q3" s="2" t="inlineStr">
         <is>
-          <t>AGGSDFGRYTYJYTUERLLFLASDKA ;L SLF'k KWE'LKWE LWQROQE</t>
-        </is>
-      </c>
+          <t>yioyio</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>yioyuio</t>
+        </is>
+      </c>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>tyrtdtj</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr"/>
+      <c r="U3" s="2" t="inlineStr"/>
+      <c r="V3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>efsf</t>
+          <t>sfgs</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>dsfds</t>
+          <t>sdfgsdf</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>dsfdf</t>
+          <t>sdfgsdf</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>sdfgsdf</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>yrtyy5</t>
+          <t>gsdfgs</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>56456456</t>
+          <t>sfg</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>t5t</t>
+          <t>sfdg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>45trgrg</t>
+          <t>sfgsadf</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>456546</t>
+          <t>sdfgs</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>ggggg</t>
+          <t>sfdgs</t>
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
         <is>
-          <t>t45t</t>
-        </is>
-      </c>
-      <c r="L4" s="3" t="inlineStr">
-        <is>
-          <t>ertretre</t>
+          <t>sfdgsdf</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>sdfgs</t>
         </is>
       </c>
       <c r="M4" s="2" t="inlineStr">
         <is>
-          <t>etretre</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="N4" s="2" t="inlineStr">
         <is>
-          <t>retertereert4tr</t>
+          <t>512 GB</t>
         </is>
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
-          <t>retertwrewrtwetr</t>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12th</t>
+        </is>
+      </c>
+      <c r="Q4" s="2" t="inlineStr">
+        <is>
+          <t>sfg</t>
+        </is>
+      </c>
+      <c r="R4" s="2" t="inlineStr">
+        <is>
+          <t>sdfgs</t>
+        </is>
+      </c>
+      <c r="S4" s="2" t="inlineStr">
+        <is>
+          <t>sdfgs</t>
+        </is>
+      </c>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>Guaya, Maleta, Teclado, Mouse, Base, Diadema</t>
+        </is>
+      </c>
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="V4" s="2" t="inlineStr">
+        <is>
+          <t>dgfhdhjfhkgh</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>23ewfew</t>
+          <t>fds</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>ewewe</t>
+          <t>fdgdfg</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>sdff</t>
+          <t>dfgdfg</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>4324e</t>
+          <t>dfgdfg</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>werewrtryey</t>
+          <t>ghhfgh</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>34545676</t>
+          <t>gfhfgh</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>er</t>
+          <t>567567657</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>erreytrui</t>
+          <t>fghgf</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>fretretr</t>
+          <t>fghfgh</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>testing</t>
+          <t>fghfghfg</t>
         </is>
       </c>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>43r34r</t>
-        </is>
-      </c>
-      <c r="L5" s="3" t="inlineStr">
-        <is>
-          <t>sf</t>
+          <t>hfghfghf</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>ghjghj</t>
         </is>
       </c>
       <c r="M5" s="2" t="inlineStr">
         <is>
-          <t>refddfg</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="N5" s="2" t="inlineStr">
         <is>
-          <t>agtryrjgloily</t>
+          <t>512 GB</t>
         </is>
       </c>
       <c r="O5" s="2" t="inlineStr">
         <is>
-          <t>fewryytjte wregwgd f erergfdgd</t>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12th</t>
+        </is>
+      </c>
+      <c r="Q5" s="2" t="inlineStr">
+        <is>
+          <t>fgfgh</t>
+        </is>
+      </c>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>fghfgh</t>
+        </is>
+      </c>
+      <c r="S5" s="2" t="inlineStr">
+        <is>
+          <t>fghfgh</t>
+        </is>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>fghfghfgh</t>
+        </is>
+      </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
+          <t>ghfdjg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>23ewfew</t>
+          <t>1 DE ENERO DE 2000</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>ewewe</t>
+          <t>CALI</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>sdff</t>
+          <t>CHIPICHAPE</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>4324e</t>
+          <t>7777</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>werewrtryey</t>
+          <t>SALA DE VENTAS</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>34545676</t>
+          <t>JUAN PEREZ</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>er</t>
+          <t>98888888</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>erreytrui</t>
+          <t>LAPTOP</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>fretretr</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>testing</t>
+          <t>440 G0</t>
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">
         <is>
-          <t>43r34r</t>
-        </is>
-      </c>
-      <c r="L6" s="3" t="inlineStr">
-        <is>
-          <t>sf</t>
+          <t>5CG343435</t>
+        </is>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>ML0001</t>
         </is>
       </c>
       <c r="M6" s="2" t="inlineStr">
         <is>
-          <t>refddfg</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="N6" s="2" t="inlineStr">
         <is>
-          <t>agtryrjgloily</t>
+          <t>512 GB</t>
         </is>
       </c>
       <c r="O6" s="2" t="inlineStr">
         <is>
-          <t>fewryytjte wregwgd f erergfdgd</t>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12th</t>
+        </is>
+      </c>
+      <c r="Q6" s="2" t="inlineStr">
+        <is>
+          <t>LG</t>
+        </is>
+      </c>
+      <c r="R6" s="2" t="inlineStr">
+        <is>
+          <t>II5I5I56</t>
+        </is>
+      </c>
+      <c r="S6" s="2" t="inlineStr">
+        <is>
+          <t>ML2323</t>
+        </is>
+      </c>
+      <c r="T6" s="2" t="inlineStr">
+        <is>
+          <t>NINGUN ACCESOSORIO</t>
+        </is>
+      </c>
+      <c r="U6" s="2" t="inlineStr">
+        <is>
+          <t>El usuario no se encuentra presente al momento de la toma de inventario.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>1 de enero de 1111</t>
+          <t>EFSFEF</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>ASDFADF</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Tintal</t>
+          <t>ASDAG</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>6666</t>
+          <t>4435</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Amanda Miguel</t>
+          <t>DSFDSF</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>9999999</t>
+          <t>EREWYTEYUTURTYU</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>LENOVO</t>
+          <t>34545664</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>THINKPAD T14</t>
+          <t>WEREWR</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>MGH4</t>
+          <t>WER</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ML4444</t>
+          <t>EWR345</t>
         </is>
       </c>
       <c r="K7" s="2" t="inlineStr">
         <is>
-          <t>SAMSUNG</t>
+          <t>DR435</t>
         </is>
       </c>
       <c r="L7" s="3" t="inlineStr">
         <is>
-          <t>S990088</t>
+          <t>TERTT</t>
         </is>
       </c>
       <c r="M7" s="2" t="inlineStr">
         <is>
-          <t>ML3333</t>
+          <t>WEER</t>
         </is>
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>SIN ACCESORIOS</t>
+          <t>34EREW</t>
         </is>
       </c>
       <c r="O7" s="2" t="inlineStr">
         <is>
-          <t>Esta es la primer acta de prueba del aplicativo de inventario y mantenimiento</t>
+          <t>SDFE45</t>
+        </is>
+      </c>
+      <c r="P7" s="2" t="inlineStr">
+        <is>
+          <t>WERRWRE</t>
+        </is>
+      </c>
+      <c r="Q7" s="2" t="inlineStr">
+        <is>
+          <t>AGGSDFGRYTYJYTUERLLFLASDKA ;L SLF'k KWE'LKWE LWQROQE</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>jdjd456</t>
+          <t>efsf</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>fkkffd</t>
+          <t>dsfds</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>dsfdf</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>sdfewrer</t>
+          <t>yrtyy5</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>56456456</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>t5t</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>45trgrg</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>456546</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>ml12345</t>
+          <t>ggggg</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
         <is>
-          <t>lf</t>
+          <t>t45t</t>
         </is>
       </c>
       <c r="L8" s="3" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>ertretre</t>
         </is>
       </c>
       <c r="M8" s="2" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>etretre</t>
         </is>
       </c>
       <c r="N8" s="2" t="inlineStr">
         <is>
-          <t>939394</t>
+          <t>retertereert4tr</t>
         </is>
       </c>
       <c r="O8" s="2" t="inlineStr">
         <is>
-          <t>dsjfhewuioi eiiewro3oi  owoeirope wpopopoer</t>
+          <t>retertwrewrtwetr</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>32423</t>
+          <t>23ewfew</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>ewqew</t>
+          <t>ewewe</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>sdff</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>4324e</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>etrtyuiuoyuiloi</t>
+          <t>werewrtryey</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>34545676</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>fh</t>
+          <t>er</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>sss</t>
+          <t>erreytrui</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>7889ppp</t>
+          <t>fretretr</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>md678</t>
+          <t>testing</t>
         </is>
       </c>
       <c r="K9" s="2" t="inlineStr">
         <is>
-          <t>jkkdfdsp</t>
+          <t>43r34r</t>
         </is>
       </c>
       <c r="L9" s="3" t="inlineStr">
         <is>
-          <t>pewpr9435</t>
+          <t>sf</t>
         </is>
       </c>
       <c r="M9" s="2" t="inlineStr">
         <is>
-          <t>sdddsf54</t>
+          <t>refddfg</t>
         </is>
       </c>
       <c r="N9" s="2" t="inlineStr">
         <is>
-          <t>dsfsfsdf</t>
+          <t>agtryrjgloily</t>
         </is>
       </c>
       <c r="O9" s="2" t="inlineStr">
         <is>
-          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
+          <t>fewryytjte wregwgd f erergfdgd</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>32423</t>
+          <t>23ewfew</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>ewqew</t>
+          <t>ewewe</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>sdff</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>4324e</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>etrtyuiuoyuiloi</t>
+          <t>werewrtryey</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>34545676</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>fh</t>
+          <t>er</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>sss</t>
+          <t>erreytrui</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>7889ppp</t>
+          <t>fretretr</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>md678</t>
+          <t>testing</t>
         </is>
       </c>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>jkkdfdsp</t>
+          <t>43r34r</t>
         </is>
       </c>
       <c r="L10" s="3" t="inlineStr">
         <is>
-          <t>pewpr9435</t>
+          <t>sf</t>
         </is>
       </c>
       <c r="M10" s="2" t="inlineStr">
         <is>
-          <t>sdddsf54</t>
+          <t>refddfg</t>
         </is>
       </c>
       <c r="N10" s="2" t="inlineStr">
         <is>
-          <t>dsfsfsdf</t>
+          <t>agtryrjgloily</t>
         </is>
       </c>
       <c r="O10" s="2" t="inlineStr">
         <is>
-          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
+          <t>fewryytjte wregwgd f erergfdgd</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>32423</t>
+          <t>1 de enero de 1111</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>ewqew</t>
+          <t>none</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>Tintal</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>6666</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>etrtyuiuoyuiloi</t>
+          <t>Amanda Miguel</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>9999999</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>fh</t>
+          <t>LENOVO</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
-          <t>sss</t>
+          <t>THINKPAD T14</t>
         </is>
       </c>
       <c r="I11" s="2" t="inlineStr">
         <is>
-          <t>7889ppp</t>
+          <t>MGH4</t>
         </is>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
-          <t>md678</t>
+          <t xml:space="preserve"> ML4444</t>
         </is>
       </c>
       <c r="K11" s="2" t="inlineStr">
         <is>
-          <t>jkkdfdsp</t>
+          <t>SAMSUNG</t>
         </is>
       </c>
       <c r="L11" s="3" t="inlineStr">
         <is>
-          <t>pewpr9435</t>
+          <t>S990088</t>
         </is>
       </c>
       <c r="M11" s="2" t="inlineStr">
         <is>
-          <t>sdddsf54</t>
+          <t>ML3333</t>
         </is>
       </c>
       <c r="N11" s="2" t="inlineStr">
         <is>
-          <t>dsfsfsdf</t>
+          <t>SIN ACCESORIOS</t>
         </is>
       </c>
       <c r="O11" s="2" t="inlineStr">
         <is>
-          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
+          <t>Esta es la primer acta de prueba del aplicativo de inventario y mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>32423</t>
+          <t>jdjd456</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>ewqew</t>
+          <t>fkkffd</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>a</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>etrtyuiuoyuiloi</t>
+          <t>sdfewrer</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
@@ -1393,47 +1517,47 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>fh</t>
+          <t>k</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>sss</t>
+          <t>e</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
-          <t>7889ppp</t>
+          <t>34</t>
         </is>
       </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>md678</t>
+          <t>ml12345</t>
         </is>
       </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
-          <t>jkkdfdsp</t>
+          <t>lf</t>
         </is>
       </c>
       <c r="L12" s="3" t="inlineStr">
         <is>
-          <t>pewpr9435</t>
+          <t>e</t>
         </is>
       </c>
       <c r="M12" s="2" t="inlineStr">
         <is>
-          <t>sdddsf54</t>
+          <t>e</t>
         </is>
       </c>
       <c r="N12" s="2" t="inlineStr">
         <is>
-          <t>dsfsfsdf</t>
+          <t>939394</t>
         </is>
       </c>
       <c r="O12" s="2" t="inlineStr">
         <is>
-          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
+          <t>dsjfhewuioi eiiewro3oi  owoeirope wpopopoer</t>
         </is>
       </c>
     </row>
@@ -1594,377 +1718,685 @@
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>ss</t>
+          <t>32423</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>sdfd</t>
+          <t>ewqew</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>erewr</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>43545</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>ferreffdvrere</t>
+          <t>etrtyuiuoyuiloi</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>4543646</t>
+          <t>987654321</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>fg</t>
+          <t>fh</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>fdgrt5</t>
+          <t>sss</t>
         </is>
       </c>
       <c r="I15" s="2" t="inlineStr">
         <is>
-          <t>ffg55789</t>
+          <t>7889ppp</t>
         </is>
       </c>
       <c r="J15" s="2" t="inlineStr">
         <is>
-          <t>md445</t>
+          <t>md678</t>
         </is>
       </c>
       <c r="K15" s="2" t="inlineStr">
         <is>
-          <t>3545</t>
+          <t>jkkdfdsp</t>
         </is>
       </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>rff45t</t>
+          <t>pewpr9435</t>
         </is>
       </c>
       <c r="M15" s="2" t="inlineStr">
         <is>
-          <t>fg565</t>
+          <t>sdddsf54</t>
         </is>
       </c>
       <c r="N15" s="2" t="inlineStr">
         <is>
-          <t>werretrtyuytuytu</t>
+          <t>dsfsfsdf</t>
         </is>
       </c>
       <c r="O15" s="2" t="inlineStr">
         <is>
-          <t>eretrefvfghytyuooiluidsvfvbvft</t>
+          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>12 de junio de 2025</t>
+          <t>32423</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>Cali</t>
+          <t>ewqew</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Jumbo</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>9333</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Juan Vega</t>
+          <t>etrtyuiuoyuiloi</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>1023458344</t>
+          <t>987654321</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>fh</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>OPTIPLEX 3540</t>
+          <t>sss</t>
         </is>
       </c>
       <c r="I16" s="2" t="inlineStr">
         <is>
-          <t>CD9934</t>
+          <t>7889ppp</t>
         </is>
       </c>
       <c r="J16" s="2" t="inlineStr">
         <is>
-          <t>ML2345</t>
+          <t>md678</t>
         </is>
       </c>
       <c r="K16" s="2" t="inlineStr">
         <is>
-          <t>LG</t>
+          <t>jkkdfdsp</t>
         </is>
       </c>
       <c r="L16" s="3" t="inlineStr">
         <is>
-          <t>L234</t>
+          <t>pewpr9435</t>
         </is>
       </c>
       <c r="M16" s="2" t="inlineStr">
         <is>
-          <t>,MD30499</t>
+          <t>sdddsf54</t>
         </is>
       </c>
       <c r="N16" s="2" t="inlineStr">
         <is>
-          <t>ML234</t>
+          <t>dsfsfsdf</t>
         </is>
       </c>
       <c r="O16" s="2" t="inlineStr">
         <is>
-          <t>TODOS</t>
-        </is>
-      </c>
-      <c r="P16" s="2" t="inlineStr">
-        <is>
-          <t>Equpo con golpe en la tapa superior</t>
+          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>se</t>
+          <t>32423</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>jj</t>
+          <t>ewqew</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>jj</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>jj</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>etrtyuiuoyuiloi</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>987654321</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>fh</t>
         </is>
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>sss</t>
         </is>
       </c>
       <c r="I17" s="2" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>7889ppp</t>
         </is>
       </c>
       <c r="J17" s="2" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>md678</t>
         </is>
       </c>
       <c r="K17" s="2" t="inlineStr">
         <is>
-          <t>oo</t>
+          <t>jkkdfdsp</t>
         </is>
       </c>
       <c r="L17" s="3" t="inlineStr">
         <is>
-          <t>oo</t>
+          <t>pewpr9435</t>
         </is>
       </c>
       <c r="M17" s="2" t="inlineStr">
         <is>
-          <t>oo</t>
+          <t>sdddsf54</t>
         </is>
       </c>
       <c r="N17" s="2" t="inlineStr">
         <is>
-          <t>oo</t>
+          <t>dsfsfsdf</t>
         </is>
       </c>
       <c r="O17" s="2" t="inlineStr">
         <is>
-          <t>llllll</t>
+          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>18 de abril 2025</t>
+          <t>32423</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>Cucuta</t>
+          <t>ewqew</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>paraiso</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>8797</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Juan Arbelaez</t>
+          <t>etrtyuiuoyuiloi</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>98789767</t>
+          <t>987654321</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>lenovo</t>
+          <t>fh</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>thinkpad t14</t>
+          <t>sss</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
-          <t>mgh4</t>
+          <t>7889ppp</t>
         </is>
       </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
-          <t>ml238903</t>
+          <t>md678</t>
         </is>
       </c>
       <c r="K18" s="2" t="inlineStr">
         <is>
-          <t>lenovo</t>
+          <t>jkkdfdsp</t>
         </is>
       </c>
       <c r="L18" s="3" t="inlineStr">
         <is>
-          <t>yhinvision u234</t>
+          <t>pewpr9435</t>
         </is>
       </c>
       <c r="M18" s="2" t="inlineStr">
         <is>
-          <t>aw9087</t>
+          <t>sdddsf54</t>
         </is>
       </c>
       <c r="N18" s="2" t="inlineStr">
         <is>
-          <t>ml38376</t>
+          <t>dsfsfsdf</t>
         </is>
       </c>
       <c r="O18" s="2" t="inlineStr">
         <is>
-          <t>guaya, maleta</t>
+          <t>aoreworwer99ewoo poewroewo wepp[peo wepoewrop[  we[poewr</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>sdfd</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>erewr</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>43545</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>ferreffdvrere</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>4543646</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>fg</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="inlineStr">
+        <is>
+          <t>fdgrt5</t>
+        </is>
+      </c>
+      <c r="I19" s="2" t="inlineStr">
+        <is>
+          <t>ffg55789</t>
+        </is>
+      </c>
+      <c r="J19" s="2" t="inlineStr">
+        <is>
+          <t>md445</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="inlineStr">
+        <is>
+          <t>3545</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>rff45t</t>
+        </is>
+      </c>
+      <c r="M19" s="2" t="inlineStr">
+        <is>
+          <t>fg565</t>
+        </is>
+      </c>
+      <c r="N19" s="2" t="inlineStr">
+        <is>
+          <t>werretrtyuytuytu</t>
+        </is>
+      </c>
+      <c r="O19" s="2" t="inlineStr">
+        <is>
+          <t>eretrefvfghytyuooiluidsvfvbvft</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>12 de junio de 2025</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>9333</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>Juan Vega</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>1023458344</t>
+        </is>
+      </c>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>DELL</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>OPTIPLEX 3540</t>
+        </is>
+      </c>
+      <c r="I20" s="2" t="inlineStr">
+        <is>
+          <t>CD9934</t>
+        </is>
+      </c>
+      <c r="J20" s="2" t="inlineStr">
+        <is>
+          <t>ML2345</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="inlineStr">
+        <is>
+          <t>LG</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>L234</t>
+        </is>
+      </c>
+      <c r="M20" s="2" t="inlineStr">
+        <is>
+          <t>,MD30499</t>
+        </is>
+      </c>
+      <c r="N20" s="2" t="inlineStr">
+        <is>
+          <t>ML234</t>
+        </is>
+      </c>
+      <c r="O20" s="2" t="inlineStr">
+        <is>
+          <t>TODOS</t>
+        </is>
+      </c>
+      <c r="P20" s="2" t="inlineStr">
+        <is>
+          <t>Equpo con golpe en la tapa superior</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>jj</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>jj</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>jj</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="H21" s="2" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="I21" s="2" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="J21" s="2" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="M21" s="2" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="N21" s="2" t="inlineStr">
+        <is>
+          <t>oo</t>
+        </is>
+      </c>
+      <c r="O21" s="2" t="inlineStr">
+        <is>
+          <t>llllll</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>18 de abril 2025</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>paraiso</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>8797</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>Juan Arbelaez</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>98789767</t>
+        </is>
+      </c>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>lenovo</t>
+        </is>
+      </c>
+      <c r="H22" s="2" t="inlineStr">
+        <is>
+          <t>thinkpad t14</t>
+        </is>
+      </c>
+      <c r="I22" s="2" t="inlineStr">
+        <is>
+          <t>mgh4</t>
+        </is>
+      </c>
+      <c r="J22" s="2" t="inlineStr">
+        <is>
+          <t>ml238903</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="inlineStr">
+        <is>
+          <t>lenovo</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>yhinvision u234</t>
+        </is>
+      </c>
+      <c r="M22" s="2" t="inlineStr">
+        <is>
+          <t>aw9087</t>
+        </is>
+      </c>
+      <c r="N22" s="2" t="inlineStr">
+        <is>
+          <t>ml38376</t>
+        </is>
+      </c>
+      <c r="O22" s="2" t="inlineStr">
+        <is>
+          <t>guaya, maleta</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
           <t>dsfsd</t>
         </is>
       </c>
-      <c r="B19" s="2" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>32e3e</t>
         </is>
       </c>
-      <c r="C19" s="2" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>332234</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>dssdfsfs</t>
         </is>
       </c>
-      <c r="E19" s="2" t="inlineStr">
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>23432</t>
         </is>
       </c>
-      <c r="F19" s="2" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>ewe</t>
         </is>
       </c>
-      <c r="G19" s="2" t="inlineStr">
+      <c r="G23" s="2" t="inlineStr">
         <is>
           <t>ewwerwe</t>
         </is>
       </c>
-      <c r="H19" s="2" t="inlineStr">
+      <c r="H23" s="2" t="inlineStr">
         <is>
           <t>werwet3</t>
         </is>
       </c>
-      <c r="I19" s="2" t="inlineStr">
+      <c r="I23" s="2" t="inlineStr">
         <is>
           <t>423rr</t>
         </is>
       </c>
-      <c r="J19" s="2" t="inlineStr">
+      <c r="J23" s="2" t="inlineStr">
         <is>
           <t>ewr2323ewrw</t>
         </is>
       </c>
-      <c r="L19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="L20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="L21" s="4" t="n"/>
-    </row>
-    <row r="22">
-      <c r="L22" s="4" t="n"/>
+      <c r="L23" s="4" t="n"/>
+    </row>
+    <row r="24">
+      <c r="L24" s="4" t="n"/>
+    </row>
+    <row r="25">
+      <c r="L25" s="4" t="n"/>
+    </row>
+    <row r="26">
+      <c r="L26" s="4" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O1"/>

</xml_diff>